<commit_message>
feat: add req 7
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -299,7 +299,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,6 +317,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -425,14 +431,14 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1317,7 +1323,7 @@
       <c r="Z11" s="6"/>
       <c r="AA11" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="14"/>
       <c r="B12" s="6"/>
       <c r="C12" s="14"/>
@@ -1346,7 +1352,7 @@
       <c r="Z12" s="6"/>
       <c r="AA12" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
         <v>62</v>
       </c>
@@ -1387,7 +1393,7 @@
       <c r="Z13" s="6"/>
       <c r="AA13" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="8">
         <v>1</v>
       </c>
@@ -1428,7 +1434,7 @@
       <c r="Z14" s="6"/>
       <c r="AA14" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="8">
         <v>2</v>
       </c>
@@ -1469,7 +1475,7 @@
       <c r="Z15" s="6"/>
       <c r="AA15" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="8">
         <v>3</v>
       </c>
@@ -1510,7 +1516,7 @@
       <c r="Z16" s="6"/>
       <c r="AA16" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="8">
         <v>4</v>
       </c>
@@ -1551,7 +1557,7 @@
       <c r="Z17" s="6"/>
       <c r="AA17" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="8">
         <v>5</v>
       </c>
@@ -1592,7 +1598,7 @@
       <c r="Z18" s="6"/>
       <c r="AA18" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="8">
         <v>6</v>
       </c>
@@ -1633,7 +1639,7 @@
       <c r="Z19" s="6"/>
       <c r="AA19" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="8">
         <v>7</v>
       </c>
@@ -1674,7 +1680,7 @@
       <c r="Z20" s="6"/>
       <c r="AA20" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="8">
         <v>8</v>
       </c>
@@ -1715,7 +1721,7 @@
       <c r="Z21" s="6"/>
       <c r="AA21" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="14"/>
       <c r="B22" s="6"/>
       <c r="C22" s="14"/>
@@ -1744,7 +1750,7 @@
       <c r="Z22" s="6"/>
       <c r="AA22" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="14"/>
       <c r="B23" s="6"/>
       <c r="C23" s="14"/>
@@ -1773,7 +1779,7 @@
       <c r="Z23" s="6"/>
       <c r="AA23" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="14"/>
       <c r="B24" s="6"/>
       <c r="C24" s="14"/>
@@ -1802,7 +1808,7 @@
       <c r="Z24" s="6"/>
       <c r="AA24" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="14"/>
       <c r="B25" s="6"/>
       <c r="C25" s="14"/>
@@ -1831,7 +1837,7 @@
       <c r="Z25" s="6"/>
       <c r="AA25" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="14"/>
       <c r="B26" s="6"/>
       <c r="C26" s="14"/>

</xml_diff>